<commit_message>
New lab results code update
Code update to also include the latest lab results from soil B. Some minor additions to X_library are also included where e.g. functions and classes got descriptions and type hints where it was missing.
</commit_message>
<xml_diff>
--- a/laboratory/LabResults.xlsx
+++ b/laboratory/LabResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ngio365-my.sharepoint.com/personal/georg_erharter_ngi_no/Documents/Research/Internal_Funding/GBV_GrainSizes/sieve_analyses/laboratory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{0762763C-7AD7-469C-BF1D-B21DB9FB1A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A57B07B2-693E-42B9-ACBB-01916B1012E7}"/>
+  <xr:revisionPtr revIDLastSave="292" documentId="8_{0762763C-7AD7-469C-BF1D-B21DB9FB1A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBC8BBD2-35E3-4346-B47F-DDB106E0384C}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{FA804907-0E07-4C33-AE1E-A73E82482871}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{FA804907-0E07-4C33-AE1E-A73E82482871}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Dry mass</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Sieve size Ø [mm]</t>
   </si>
@@ -111,6 +108,18 @@
   </si>
   <si>
     <t>Cu</t>
+  </si>
+  <si>
+    <t>Soil B (ISO)</t>
+  </si>
+  <si>
+    <t>Dry mass [g]</t>
+  </si>
+  <si>
+    <t>Soil B (1000g)</t>
+  </si>
+  <si>
+    <t>Soil B (300g)</t>
   </si>
 </sst>
 </file>
@@ -350,6 +359,21 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,21 +381,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -709,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA8D491-5DCF-4B6E-B1C5-698F3C2B2B1E}">
-  <dimension ref="B1:K54"/>
+  <dimension ref="B1:N54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,340 +729,412 @@
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="19.28515625" style="3" customWidth="1"/>
-    <col min="12" max="26" width="19.28515625" customWidth="1"/>
+    <col min="4" max="14" width="19.28515625" style="3" customWidth="1"/>
+    <col min="15" max="29" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="25" t="s">
+      <c r="L3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>90</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27">
+      <c r="K4" s="3">
         <v>100</v>
       </c>
-      <c r="I4" s="6">
+      <c r="L4" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>63</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27">
+      <c r="K5" s="3">
         <v>96</v>
       </c>
-      <c r="I5" s="6">
+      <c r="L5" s="6">
         <v>96.8</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>45</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27">
+      <c r="K6" s="3">
         <v>91</v>
       </c>
-      <c r="I6" s="6">
+      <c r="L6" s="6">
         <v>89.9</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>31.5</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27">
+      <c r="H7" s="3">
+        <v>100</v>
+      </c>
+      <c r="I7" s="3">
+        <v>100</v>
+      </c>
+      <c r="J7" s="3">
+        <v>100</v>
+      </c>
+      <c r="K7" s="3">
         <v>83.6</v>
       </c>
-      <c r="I7" s="6">
+      <c r="L7" s="6">
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>16</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27">
+      <c r="H8" s="3">
+        <v>95.65</v>
+      </c>
+      <c r="I8" s="3">
+        <v>95.08</v>
+      </c>
+      <c r="J8" s="3">
+        <v>96.36</v>
+      </c>
+      <c r="K8" s="3">
         <v>64.400000000000006</v>
       </c>
-      <c r="I8" s="6">
+      <c r="L8" s="6">
         <v>56.6</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>8</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27">
+      <c r="H9" s="3">
+        <v>84.46</v>
+      </c>
+      <c r="I9" s="3">
+        <v>85.8</v>
+      </c>
+      <c r="J9" s="3">
+        <v>92.23</v>
+      </c>
+      <c r="K9" s="3">
         <v>45.2</v>
       </c>
-      <c r="I9" s="6">
+      <c r="L9" s="6">
         <v>38.9</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>4</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="3">
         <v>100</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="3">
         <v>100</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="3">
         <v>100</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="3">
         <v>100</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="3">
         <v>100</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="3">
+        <v>65.08</v>
+      </c>
+      <c r="I10" s="3">
+        <v>66.37</v>
+      </c>
+      <c r="J10" s="3">
+        <v>77.42</v>
+      </c>
+      <c r="K10" s="3">
         <v>31.3</v>
       </c>
-      <c r="I10" s="6">
+      <c r="L10" s="6">
         <v>26.4</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>2</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="3">
         <v>99.79</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="3">
         <v>99.69</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="3">
         <v>99.88</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="3">
         <v>99.74</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="3">
         <v>99.2</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H11" s="3">
+        <v>38.67</v>
+      </c>
+      <c r="I11" s="3">
+        <v>39.44</v>
+      </c>
+      <c r="J11" s="3">
+        <v>48.81</v>
+      </c>
+      <c r="K11" s="3">
         <v>22.8</v>
       </c>
-      <c r="I11" s="6">
+      <c r="L11" s="6">
         <v>19.2</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>1</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="3">
         <v>98.99</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="3">
         <v>99.04</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="3">
         <v>99.16</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="3">
         <v>99.1</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="3">
         <v>98.8</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="3">
+        <v>19.079999999999998</v>
+      </c>
+      <c r="I12" s="3">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="J12" s="3">
+        <v>23.88</v>
+      </c>
+      <c r="K12" s="3">
         <v>15.8</v>
       </c>
-      <c r="I12" s="6">
+      <c r="L12" s="6">
         <v>13.5</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>0.5</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="3">
         <v>94.29</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="3">
         <v>94.89</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="3">
         <v>94.26</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="3">
         <v>95.42</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="3">
         <v>94.4</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="3">
+        <v>7.77</v>
+      </c>
+      <c r="I13" s="3">
+        <v>7.49</v>
+      </c>
+      <c r="J13" s="3">
+        <v>8.35</v>
+      </c>
+      <c r="K13" s="3">
         <v>11.1</v>
       </c>
-      <c r="I13" s="6">
+      <c r="L13" s="6">
         <v>9.5</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>0.25</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="3">
         <v>64.92</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="3">
         <v>68.239999999999995</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="3">
         <v>62.89</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="3">
         <v>68.099999999999994</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="3">
         <v>66.400000000000006</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="3">
+        <v>2.54</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2.35</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2.37</v>
+      </c>
+      <c r="K14" s="3">
         <v>9</v>
       </c>
-      <c r="I14" s="6">
+      <c r="L14" s="6">
         <v>7.7</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>0.125</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="3">
         <v>22.32</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="3">
         <v>22.76</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="3">
         <v>18.350000000000001</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="3">
         <v>24.7</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="3">
         <v>26.2</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="K15" s="3">
         <v>7.8</v>
       </c>
-      <c r="I15" s="6">
+      <c r="L15" s="6">
         <v>6.8</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>6.3E-2</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="24">
         <v>4.97</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="24">
         <v>2.74</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="24">
         <v>3.72</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="24">
         <v>3.26</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="24">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="29"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I16" s="24">
+        <v>0.31</v>
+      </c>
+      <c r="J16" s="24">
+        <v>0.27</v>
+      </c>
+      <c r="K16" s="24"/>
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3">
         <v>200</v>
@@ -1070,16 +1151,25 @@
       <c r="G17" s="3">
         <v>5</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="3">
+        <v>9000</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1000</v>
+      </c>
+      <c r="J17" s="3">
+        <v>300</v>
+      </c>
+      <c r="K17" s="15">
         <v>50000</v>
       </c>
-      <c r="I17" s="16">
+      <c r="L17" s="16">
         <v>20000</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="12">
         <f>D17/$C$17</f>
@@ -1097,14 +1187,23 @@
         <f>G17/$C$17</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I18" s="17">
-        <f>I17/H17</f>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12">
+        <f>I17/$H$17</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J18" s="12">
+        <f>J17/$H$17</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="L18" s="17">
+        <f>L17/K17</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="20">
         <f>_xlfn.FORECAST.LINEAR(10,$B15:$B16,C15:C16)</f>
@@ -1127,17 +1226,29 @@
         <v>7.8926605504587161E-2</v>
       </c>
       <c r="H19" s="20">
-        <f>_xlfn.FORECAST.LINEAR(10,$B13:$B14,H13:H14)</f>
+        <f>_xlfn.FORECAST.LINEAR(10,$B12:$B13,H12:H13)</f>
+        <v>0.59858532272325382</v>
+      </c>
+      <c r="I19" s="20">
+        <f>_xlfn.FORECAST.LINEAR(10,$B12:$B13,I12:I13)</f>
+        <v>0.60809646856158484</v>
+      </c>
+      <c r="J19" s="20">
+        <f>_xlfn.FORECAST.LINEAR(10,$B12:$B13,J12:J13)</f>
+        <v>0.55312298776561497</v>
+      </c>
+      <c r="K19" s="20">
+        <f>_xlfn.FORECAST.LINEAR(10,$B13:$B14,K13:K14)</f>
         <v>0.36904761904761907</v>
       </c>
-      <c r="I19" s="21">
-        <f>_xlfn.FORECAST.LINEAR(10,$B12:$B13,I12:I13)</f>
+      <c r="L19" s="21">
+        <f>_xlfn.FORECAST.LINEAR(10,$B12:$B13,L12:L13)</f>
         <v>0.5625</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="20">
         <f>_xlfn.FORECAST.LINEAR(30,$B14:$B15,C14:C15)</f>
@@ -1160,17 +1271,29 @@
         <v>0.13681592039800994</v>
       </c>
       <c r="H20" s="20">
-        <f>_xlfn.FORECAST.LINEAR(30,$B10:$B11,H10:H11)</f>
+        <f>_xlfn.FORECAST.LINEAR(30,$B11:$B12,H11:H12)</f>
+        <v>1.5574272588055129</v>
+      </c>
+      <c r="I20" s="20">
+        <f>_xlfn.FORECAST.LINEAR(30,$B11:$B12,I11:I12)</f>
+        <v>1.5358898721730581</v>
+      </c>
+      <c r="J20" s="20">
+        <f t="shared" ref="J20" si="0">_xlfn.FORECAST.LINEAR(30,$B11:$B12,J11:J12)</f>
+        <v>1.2454873646209388</v>
+      </c>
+      <c r="K20" s="20">
+        <f>_xlfn.FORECAST.LINEAR(30,$B10:$B11,K10:K11)</f>
         <v>3.6941176470588228</v>
       </c>
-      <c r="I20" s="21">
-        <f>_xlfn.FORECAST.LINEAR(30,$B9:$B10,I9:I10)</f>
+      <c r="L20" s="21">
+        <f>_xlfn.FORECAST.LINEAR(30,$B9:$B10,L9:L10)</f>
         <v>5.1519999999999992</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="20">
         <f>_xlfn.FORECAST.LINEAR(60,$B14:$B15,C14:C15)</f>
@@ -1193,147 +1316,219 @@
         <v>0.23009950248756217</v>
       </c>
       <c r="H21" s="20">
-        <f>_xlfn.FORECAST.LINEAR(60,$B8:$B9,H8:H9)</f>
+        <f>_xlfn.FORECAST.LINEAR(60,$B10:$B11,H10:H11)</f>
+        <v>3.6152972358954947</v>
+      </c>
+      <c r="I21" s="20">
+        <f t="shared" ref="I21:J21" si="1">_xlfn.FORECAST.LINEAR(60,$B10:$B11,I10:I11)</f>
+        <v>3.5269216487189006</v>
+      </c>
+      <c r="J21" s="20">
+        <f t="shared" si="1"/>
+        <v>2.7822439706396365</v>
+      </c>
+      <c r="K21" s="20">
+        <f>_xlfn.FORECAST.LINEAR(60,$B8:$B9,K8:K9)</f>
         <v>14.166666666666664</v>
       </c>
-      <c r="I21" s="21">
-        <f>_xlfn.FORECAST.LINEAR(60,$B7:$B8,I7:I8)</f>
+      <c r="L21" s="21">
+        <f>_xlfn.FORECAST.LINEAR(60,$B7:$B8,L7:L8)</f>
         <v>18.45116279069768</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="20">
         <f>(C20^2)/(C21*C19)</f>
         <v>1.1411285297973055</v>
       </c>
       <c r="D22" s="20">
-        <f t="shared" ref="D22:G22" si="0">(D20^2)/(D21*D19)</f>
+        <f t="shared" ref="D22:G22" si="2">(D20^2)/(D21*D19)</f>
         <v>1.0803076593731922</v>
       </c>
       <c r="E22" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1472182708760585</v>
       </c>
       <c r="F22" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.05220081513552</v>
       </c>
       <c r="G22" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.0307044906221519</v>
       </c>
       <c r="H22" s="20">
-        <f t="shared" ref="H22" si="1">(H20^2)/(H21*H19)</f>
+        <f t="shared" ref="H22:J22" si="3">(H20^2)/(H21*H19)</f>
+        <v>1.1208447718620056</v>
+      </c>
+      <c r="I22" s="20">
+        <f t="shared" si="3"/>
+        <v>1.0998966013454772</v>
+      </c>
+      <c r="J22" s="20">
+        <f t="shared" si="3"/>
+        <v>1.0080027895581589</v>
+      </c>
+      <c r="K22" s="20">
+        <f t="shared" ref="K22" si="4">(K20^2)/(K21*K19)</f>
         <v>2.6101854329855612</v>
       </c>
-      <c r="I22" s="21">
-        <f t="shared" ref="I22" si="2">(I20^2)/(I21*I19)</f>
+      <c r="L22" s="21">
+        <f t="shared" ref="L22" si="5">(L20^2)/(L21*L19)</f>
         <v>2.5574399282973403</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="20">
         <f>C21/C19</f>
         <v>2.9091006882201165</v>
       </c>
       <c r="D23" s="20">
-        <f t="shared" ref="D23:G23" si="3">D21/D19</f>
+        <f t="shared" ref="D23:G23" si="6">D21/D19</f>
         <v>2.6596084467540702</v>
       </c>
       <c r="E23" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.6992415612333334</v>
       </c>
       <c r="F23" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.7478319960436304</v>
       </c>
       <c r="G23" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.9153604290531532</v>
       </c>
       <c r="H23" s="20">
-        <f t="shared" ref="H23:I23" si="4">H21/H19</f>
+        <f t="shared" ref="H23:J23" si="7">H21/H19</f>
+        <v>6.0397358549450573</v>
+      </c>
+      <c r="I23" s="20">
+        <f t="shared" si="7"/>
+        <v>5.7999377254428381</v>
+      </c>
+      <c r="J23" s="20">
+        <f t="shared" si="7"/>
+        <v>5.0300638956965722</v>
+      </c>
+      <c r="K23" s="20">
+        <f t="shared" ref="K23:L23" si="8">K21/K19</f>
         <v>38.387096774193537</v>
       </c>
-      <c r="I23" s="21">
-        <f t="shared" si="4"/>
+      <c r="L23" s="21">
+        <f t="shared" si="8"/>
         <v>32.80206718346254</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="24"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="5">
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="29"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
         <v>90</v>
       </c>
-      <c r="I25" s="18">
-        <f t="shared" ref="I25:I37" si="5">ABS(H4-I4)</f>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="26">
+        <f t="shared" ref="L25:L37" si="9">ABS(K4-L4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
         <v>63</v>
       </c>
-      <c r="I26" s="18">
-        <f t="shared" si="5"/>
+      <c r="L26" s="18">
+        <f t="shared" si="9"/>
         <v>0.79999999999999716</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
         <v>45</v>
       </c>
-      <c r="I27" s="18">
-        <f t="shared" si="5"/>
+      <c r="L27" s="18">
+        <f t="shared" si="9"/>
         <v>1.0999999999999943</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
         <v>31.5</v>
       </c>
-      <c r="I28" s="18">
-        <f t="shared" si="5"/>
+      <c r="I28" s="3">
+        <f t="shared" ref="I28:J30" si="10">ABS(I7-$H7)</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="18">
+        <f t="shared" si="9"/>
         <v>5.5</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
         <v>16</v>
       </c>
-      <c r="I29" s="18">
-        <f t="shared" si="5"/>
+      <c r="I29" s="3">
+        <f t="shared" si="10"/>
+        <v>0.57000000000000739</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="10"/>
+        <v>0.70999999999999375</v>
+      </c>
+      <c r="L29" s="18">
+        <f t="shared" si="9"/>
         <v>7.8000000000000043</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
         <v>8</v>
       </c>
-      <c r="I30" s="18">
-        <f t="shared" si="5"/>
+      <c r="I30" s="3">
+        <f t="shared" si="10"/>
+        <v>1.3400000000000034</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="10"/>
+        <v>7.7700000000000102</v>
+      </c>
+      <c r="L30" s="18">
+        <f t="shared" si="9"/>
         <v>6.3000000000000043</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
         <v>4</v>
       </c>
@@ -1353,164 +1548,220 @@
         <f>ABS(G10-$C10)</f>
         <v>0</v>
       </c>
-      <c r="I31" s="18">
-        <f t="shared" si="5"/>
+      <c r="I31" s="3">
+        <f>ABS(I10-$H10)</f>
+        <v>1.2900000000000063</v>
+      </c>
+      <c r="J31" s="3">
+        <f>ABS(J10-$H10)</f>
+        <v>12.340000000000003</v>
+      </c>
+      <c r="L31" s="18">
+        <f t="shared" si="9"/>
         <v>4.9000000000000021</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
         <v>2</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" ref="D32:E37" si="6">ABS(D11-$C11)</f>
+        <f t="shared" ref="D32:E37" si="11">ABS(D11-$C11)</f>
         <v>0.10000000000000853</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>8.99999999999892E-2</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" ref="F32:G32" si="7">ABS(F11-$C11)</f>
+        <f t="shared" ref="F32:G32" si="12">ABS(F11-$C11)</f>
         <v>5.0000000000011369E-2</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.59000000000000341</v>
       </c>
-      <c r="I32" s="18">
-        <f t="shared" si="5"/>
+      <c r="I32" s="3">
+        <f t="shared" ref="I32:J37" si="13">ABS(I11-$H11)</f>
+        <v>0.76999999999999602</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="13"/>
+        <v>10.14</v>
+      </c>
+      <c r="L32" s="18">
+        <f t="shared" si="9"/>
         <v>3.6000000000000014</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="5">
         <v>1</v>
       </c>
       <c r="D33" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5.0000000000011369E-2</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.17000000000000171</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" ref="F33:G33" si="8">ABS(F12-$C12)</f>
+        <f t="shared" ref="F33:G33" si="14">ABS(F12-$C12)</f>
         <v>0.10999999999999943</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.18999999999999773</v>
       </c>
-      <c r="I33" s="18">
-        <f t="shared" si="5"/>
+      <c r="I33" s="3">
+        <f t="shared" si="13"/>
+        <v>2.0000000000003126E-2</v>
+      </c>
+      <c r="J33" s="3">
+        <f t="shared" si="13"/>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="L33" s="18">
+        <f t="shared" si="9"/>
         <v>2.3000000000000007</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="5">
         <v>0.5</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.59999999999999432</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3.0000000000001137E-2</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" ref="F34:G34" si="9">ABS(F13-$C13)</f>
+        <f t="shared" ref="F34:G34" si="15">ABS(F13-$C13)</f>
         <v>1.1299999999999955</v>
       </c>
       <c r="G34" s="3">
+        <f t="shared" si="15"/>
+        <v>0.10999999999999943</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="13"/>
+        <v>0.27999999999999936</v>
+      </c>
+      <c r="J34" s="3">
+        <f t="shared" si="13"/>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="L34" s="18">
         <f t="shared" si="9"/>
-        <v>0.10999999999999943</v>
-      </c>
-      <c r="I34" s="18">
-        <f t="shared" si="5"/>
         <v>1.5999999999999996</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="5">
         <v>0.25</v>
       </c>
       <c r="D35" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3.3199999999999932</v>
       </c>
       <c r="E35" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2.0300000000000011</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" ref="F35:G35" si="10">ABS(F14-$C14)</f>
+        <f t="shared" ref="F35:G35" si="16">ABS(F14-$C14)</f>
         <v>3.1799999999999926</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1.480000000000004</v>
       </c>
-      <c r="I35" s="18">
-        <f t="shared" si="5"/>
+      <c r="I35" s="3">
+        <f t="shared" si="13"/>
+        <v>0.18999999999999995</v>
+      </c>
+      <c r="J35" s="3">
+        <f t="shared" si="13"/>
+        <v>0.16999999999999993</v>
+      </c>
+      <c r="L35" s="18">
+        <f t="shared" si="9"/>
         <v>1.2999999999999998</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="5">
         <v>0.125</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.44000000000000128</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3.9699999999999989</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" ref="F36:G36" si="11">ABS(F15-$C15)</f>
+        <f t="shared" ref="F36:G36" si="17">ABS(F15-$C15)</f>
         <v>2.379999999999999</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>3.879999999999999</v>
       </c>
-      <c r="I36" s="18">
-        <f t="shared" si="5"/>
+      <c r="I36" s="3">
+        <f t="shared" si="13"/>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="J36" s="3">
+        <f t="shared" si="13"/>
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="L36" s="18">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="5">
         <v>6.3E-2</v>
       </c>
       <c r="D37" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2.2299999999999995</v>
       </c>
       <c r="E37" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.2499999999999996</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" ref="F37:G37" si="12">ABS(F16-$C16)</f>
+        <f t="shared" ref="F37:G37" si="18">ABS(F16-$C16)</f>
         <v>1.71</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.5699999999999994</v>
       </c>
-      <c r="I37" s="18">
-        <f t="shared" si="5"/>
+      <c r="I37" s="3">
+        <f t="shared" si="13"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="J37" s="3">
+        <f t="shared" si="13"/>
+        <v>1.9999999999999962E-2</v>
+      </c>
+      <c r="L37" s="18">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="9">
@@ -1518,24 +1769,33 @@
         <v>3.3199999999999932</v>
       </c>
       <c r="E38" s="9">
-        <f t="shared" ref="E38:G38" si="13">MAX(E25:E37)</f>
+        <f t="shared" ref="E38:J38" si="19">MAX(E25:E37)</f>
         <v>3.9699999999999989</v>
       </c>
       <c r="F38" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>3.1799999999999926</v>
       </c>
       <c r="G38" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>3.879999999999999</v>
       </c>
-      <c r="H38" s="19"/>
-      <c r="I38" s="10">
-        <f>MAX(I25:I37)</f>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9">
+        <f t="shared" si="19"/>
+        <v>1.3400000000000034</v>
+      </c>
+      <c r="J38" s="9">
+        <f t="shared" si="19"/>
+        <v>12.340000000000003</v>
+      </c>
+      <c r="K38" s="19"/>
+      <c r="L38" s="10">
+        <f>MAX(L25:L37)</f>
         <v>7.8000000000000043</v>
       </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C49" s="2"/>
@@ -1580,7 +1840,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B24:L24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>